<commit_message>
Add deer & wolf
</commit_message>
<xml_diff>
--- a/Assets/Guide/StatData.xlsx
+++ b/Assets/Guide/StatData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\DAWN\Assets\Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840B58D9-2A6C-4E78-A6BE-BB3B738EC4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E2709F-4E34-4BF2-AD4F-F4838AF4B989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{71E63FF0-473D-41DB-B7B2-B2B736103E75}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t>Ton</t>
   </si>
@@ -70,30 +70,6 @@
     <t>HP: 80; DMG: 6; Spd: 6; SkillCD: 5; Shield: 50; AtkSpd: 7</t>
   </si>
   <si>
-    <t>HP: 15-30; DMG: 10-25; Spd: 5-14; SkillCD: 0; Shield: 10; AtkSpd: 0</t>
-  </si>
-  <si>
-    <t>HP: 15; DMG: 2-6; Spd: 10-20; SkillCD: 8-14; Shield: 0-20; AtkSpd: 8-17</t>
-  </si>
-  <si>
-    <t>HP: 15; DMG: 2-6; Spd: 10-20; SkillCD: 8-14; Shield: 0-20; AtkSpd: 8-18</t>
-  </si>
-  <si>
-    <t>HP: 15; DMG: 2-6; Spd: 10-20; SkillCD: 8-14; Shield: 0-20; AtkSpd: 8-19</t>
-  </si>
-  <si>
-    <t>HP: 15-30; DMG: 10-25; Spd: 5-14; SkillCD: 0; Shield: 10; AtkSpd: 1</t>
-  </si>
-  <si>
-    <t>HP: 15-30; DMG: 10-25; Spd: 5-14; SkillCD: 0; Shield: 10; AtkSpd: 2</t>
-  </si>
-  <si>
-    <t>HP: 15-30; DMG: 10-25; Spd: 5-14; SkillCD: 0; Shield: 10; AtkSpd: 3</t>
-  </si>
-  <si>
-    <t>HP: 15-30; DMG: 10-25; Spd: 5-14; SkillCD: 0; Shield: 10; AtkSpd: 4</t>
-  </si>
-  <si>
     <t>HP: 6; DMG: 6; Spd: 8; SkillCD: 20; Shield: 3; AtkSpd: 5</t>
   </si>
   <si>
@@ -236,13 +212,97 @@
   </si>
   <si>
     <t>Fortress(T1)</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>HP: 15; DMG: 2; Spd: 12; SkillCD: 10; Shield: 0; AtkSpd: 9</t>
+  </si>
+  <si>
+    <t>HP: 15; DMG: 2; Spd: 14; SkillCD: 12; Shield: 5; AtkSpd: 12</t>
+  </si>
+  <si>
+    <t>HP: 15; DMG: 4; Spd: 16; SkillCD: 12; Shield: 10; AtkSpd: 12</t>
+  </si>
+  <si>
+    <t>HP: 15; DMG: 10; Spd: 5; SkillCD: 0; Shield: 10; AtkSpd: 0</t>
+  </si>
+  <si>
+    <t>HP: 30; DMG: 25; Spd: 14; SkillCD: 0; Shield: 10; AtkSpd: 4</t>
+  </si>
+  <si>
+    <t>HP: 20; DMG: 15; Spd: 10; SkillCD: 0; Shield: 10; AtkSpd: 1</t>
+  </si>
+  <si>
+    <t>HP: 20; DMG: 20; Spd: 10; SkillCD: 0; Shield: 10; AtkSpd: 2</t>
+  </si>
+  <si>
+    <t>HP: 25; DMG: 20; Spd: 10; SkillCD: 0; Shield: 10; AtkSpd: 3</t>
+  </si>
+  <si>
+    <t>HP: 20; DMG: 2; Spd: 4; SkillCD: 12; Shield: 10; AtkSpd: 2</t>
+  </si>
+  <si>
+    <t>HP: 90; DMG: 6; Spd: 4; SkillCD: 6; Shield: 30; AtkSpd: 4</t>
+  </si>
+  <si>
+    <t>HP: 55; DMG: 5; Spd: 4; SkillCD: 8; Shield: 25; AtkSpd: 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 45; DMG: 4; Spd: 4; SkillCD: 10; Shield: 20; AtkSpd: 3</t>
+  </si>
+  <si>
+    <t>HP: 36; DMG: 3; Spd: 4; SkillCD: 10; Shield: 15; AtkSpd: 2</t>
+  </si>
+  <si>
+    <t>HP: 20; DMG: 4; Spd: 10; SkillCD: 18; Shield: 10; AtkSpd: 5</t>
+  </si>
+  <si>
+    <t>HP: 30; DMG: 6; Spd: 11; SkillCD: 16; Shield: 15; AtkSpd: 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 40; DMG: 8; Spd: 12; SkillCD: 14; Shield: 20; AtkSpd: 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 50; DMG: 10; Spd: 13; SkillCD: 12; Shield: 25; AtkSpd: 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 60; DMG: 12; Spd: 14; SkillCD: 10; Shield: 30; AtkSpd: 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 10; DMG: 6; Spd: 12; SkillCD: 16; Shield: 2; AtkSpd: 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 15; DMG: 8; Spd: 14; SkillCD: 14; Shield: 4; AtkSpd: 7</t>
+  </si>
+  <si>
+    <t>HP: 20; DMG: 10; Spd: 16; SkillCD: 12; Shield: 6; AtkSpd: 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 25; DMG: 12; Spd: 18; SkillCD: 10; Shield: 8; AtkSpd: 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	HP: 30; DMG: 15; Spd: 20; SkillCD: 8; Shield: 10; AtkSpd: 20</t>
+  </si>
+  <si>
+    <t>ALLY</t>
+  </si>
+  <si>
+    <t>Enemy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +336,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6161"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,26 +394,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6161"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -649,20 +734,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DEEF68-2B08-495F-A0B1-0D9549A78973}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="134.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="137" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -679,85 +765,151 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="H1" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="H2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
+      <c r="B5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -770,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1B08B2-5CFE-4465-BA25-998B282FF49B}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,467 +954,467 @@
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="2">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4">
         <v>-100</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>-20</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>-10</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>46</v>
+      <c r="K2" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
         <v>-50</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>-10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>-5</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
         <v>-10</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="K3" s="10" t="s">
-        <v>63</v>
+      <c r="K3" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4">
         <v>-120</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>-50</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>-10</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <v>-20</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4">
         <v>-20</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
         <v>-3</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>-10</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>65</v>
+      <c r="G5" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="2">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4">
         <v>-50</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>-30</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>-3</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5"/>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4">
         <v>-70</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>-10</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>-3</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5"/>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4">
         <v>-100</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>-60</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>-5</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
         <v>-5</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5">
         <v>30</v>
       </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="5">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>10</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>20</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="6">
+        <v>-10</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-10</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-10</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-20</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="6">
+        <v>-5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-15</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="2">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>20</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" s="2">
-        <v>-10</v>
-      </c>
-      <c r="C17" s="2">
-        <v>-5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="2">
-        <v>-10</v>
-      </c>
-      <c r="C18" s="2">
-        <v>-10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="2">
-        <v>-20</v>
-      </c>
-      <c r="C19" s="2">
-        <v>-5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="2">
-        <v>-5</v>
-      </c>
-      <c r="C21" s="2">
-        <v>-15</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- update data for Q-Learning
</commit_message>
<xml_diff>
--- a/Assets/Guide/StatData.xlsx
+++ b/Assets/Guide/StatData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\DAWN\Assets\Guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Project_DAWN\Assets\Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B35BFED-76B9-4CC3-AC9F-C42ABF45A82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB5237-2C4B-49EC-BE1F-504E56BD46EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{71E63FF0-473D-41DB-B7B2-B2B736103E75}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{71E63FF0-473D-41DB-B7B2-B2B736103E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Stat" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -476,12 +479,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,9 +509,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -546,7 +549,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -652,7 +655,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -794,7 +797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DEEF68-2B08-495F-A0B1-0D9549A78973}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1185,7 @@
       <c r="F5" s="4">
         <v>-10</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1205,7 +1208,7 @@
       <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -1226,7 +1229,7 @@
       <c r="F7" s="4">
         <v>0</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -1461,7 +1464,7 @@
       <c r="E1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="14"/>
       <c r="P1" s="9" t="s">
         <v>55</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -1506,7 +1509,7 @@
       <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -1527,7 +1530,7 @@
       <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
@@ -1548,7 +1551,7 @@
       <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
@@ -1571,11 +1574,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="6" t="s">
         <v>58</v>
       </c>

</xml_diff>